<commit_message>
added pasport number filing
</commit_message>
<xml_diff>
--- a/patients.xlsx
+++ b/patients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Фамилия</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Дата выдачи</t>
+  </si>
+  <si>
+    <t>8673515150</t>
   </si>
 </sst>
 </file>
@@ -121,11 +124,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -425,7 +431,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -434,7 +440,7 @@
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -460,7 +466,7 @@
       <c r="G1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="3" t="s">
@@ -489,6 +495,9 @@
       <c r="F2">
         <v>10000</v>
       </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
@@ -509,6 +518,9 @@
       <c r="F3">
         <v>99</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
@@ -529,6 +541,9 @@
       <c r="F4">
         <v>123</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
@@ -548,6 +563,9 @@
       </c>
       <c r="F5">
         <v>1234</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added reference_number filling and changed file patients.xlsx
</commit_message>
<xml_diff>
--- a/patients.xlsx
+++ b/patients.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Фамилия</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>581702534850</t>
+  </si>
+  <si>
+    <t>Номер справки</t>
   </si>
 </sst>
 </file>
@@ -127,14 +130,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -431,167 +431,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>3334</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
-        <v>31689</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
+        <v>31689</v>
+      </c>
+      <c r="F2" s="2">
         <v>2024</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>10000</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>31689</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>3335</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1">
-        <v>31689</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
+        <v>31689</v>
+      </c>
+      <c r="F3" s="2">
         <v>2023</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>99</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>31689</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>3336</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="1">
-        <v>31689</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
+        <v>31689</v>
+      </c>
+      <c r="F4" s="2">
         <v>2024</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>123</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>31689</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>3337</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1">
-        <v>31689</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
+        <v>31689</v>
+      </c>
+      <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>1234</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>31689</v>
       </c>
     </row>

</xml_diff>